<commit_message>
big improvement: add flash read/write
</commit_message>
<xml_diff>
--- a/DOC/flash分配.xlsx
+++ b/DOC/flash分配.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
   <si>
     <t>全局变量</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,10 +75,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MSA0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>基地址</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -178,6 +174,65 @@
   </si>
   <si>
     <t>0x1C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Light_threshold1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Light_threshold2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Light_threshold3</t>
+  </si>
+  <si>
+    <t>Light_threshold4</t>
+  </si>
+  <si>
+    <t>0x2C</t>
+  </si>
+  <si>
+    <t>0x20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>光敏门限1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>光敏门限2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>光敏门限3</t>
+  </si>
+  <si>
+    <t>光敏门限4</t>
+  </si>
+  <si>
+    <t>u32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delay_time_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>延时感应时间设置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x30</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -242,7 +297,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -256,6 +311,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -557,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -589,13 +647,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -603,13 +661,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>13</v>
@@ -626,19 +684,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="3">
         <v>32</v>
@@ -649,19 +707,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="G4" s="3">
         <v>3</v>
@@ -672,19 +730,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
@@ -695,19 +753,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="G6" s="3">
         <v>40</v>
@@ -718,19 +776,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="G7" s="3">
         <v>6</v>
@@ -741,19 +799,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="E8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="3">
         <v>60</v>
@@ -764,85 +822,180 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G9" s="3">
         <v>0.6</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="E10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
       <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="5">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="5">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
+      <c r="F15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="3"/>
+      <c r="B16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update new parameter and fix some typo, but not test
</commit_message>
<xml_diff>
--- a/DOC/flash分配.xlsx
+++ b/DOC/flash分配.xlsx
@@ -618,7 +618,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -676,7 +676,7 @@
         <v>11</v>
       </c>
       <c r="G2" s="3">
-        <v>4</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -699,7 +699,7 @@
         <v>16</v>
       </c>
       <c r="G3" s="3">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -722,7 +722,7 @@
         <v>24</v>
       </c>
       <c r="G4" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -745,7 +745,7 @@
         <v>25</v>
       </c>
       <c r="G5" s="3">
-        <v>4</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -768,7 +768,7 @@
         <v>29</v>
       </c>
       <c r="G6" s="3">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -791,7 +791,7 @@
         <v>34</v>
       </c>
       <c r="G7" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -814,7 +814,7 @@
         <v>39</v>
       </c>
       <c r="G8" s="3">
-        <v>60</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -837,7 +837,7 @@
         <v>40</v>
       </c>
       <c r="G9" s="3">
-        <v>0.6</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="10" spans="1:7">

</xml_diff>

<commit_message>
basic complete code for the serial protocol v1.11
</commit_message>
<xml_diff>
--- a/DOC/flash分配.xlsx
+++ b/DOC/flash分配.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="16155" windowHeight="8505"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="16157" windowHeight="8503"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
   <si>
     <t>全局变量</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -233,6 +233,58 @@
   </si>
   <si>
     <t>0x30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delay_time_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感应延时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>秒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>flash_def.h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>protocol.c:reset_default_parameter()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>protocol.h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>毫秒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main.c:set_var_from_flash() and save_upssa0()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通讯周期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>upload_duty</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -615,25 +667,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="11.73046875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.9296875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.73046875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.1328125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.53125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.19921875" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.06640625" style="2"/>
+    <col min="1" max="1" width="11.69140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.23046875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.921875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.69140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.15234375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.53515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.23046875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.69140625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.07421875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -656,7 +709,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -679,7 +732,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -702,7 +755,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -725,7 +778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -748,7 +801,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -771,7 +824,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -794,7 +847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -817,7 +870,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -840,7 +893,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -863,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -886,7 +939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -909,7 +962,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -932,69 +985,141 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7">
+        <v>58</v>
+      </c>
+      <c r="G14" s="5">
+        <v>32</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="G15" s="5">
+        <v>8000</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G18" s="5">
         <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="I19" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="I20" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="I21" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="I22" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fresh new parameter from sz
</commit_message>
<xml_diff>
--- a/DOC/flash分配.xlsx
+++ b/DOC/flash分配.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
   <si>
     <t>全局变量</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -260,31 +260,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>protocol.h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>毫秒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通讯周期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>upload_duty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>load_ceiling_setup()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main.c:set_var_from_flash() and save_upssa0()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>load_ceiling_setup(0);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>protocol.c:reset_default_parameter()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>protocol.h</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>毫秒</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x34</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>main.c:set_var_from_flash() and save_upssa0()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>通讯周期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>upload_duty</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -295,7 +303,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.000_ "/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,6 +319,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -320,7 +336,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -343,13 +359,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -366,6 +432,18 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -667,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="14.15"/>
@@ -686,7 +764,7 @@
     <col min="9" max="16384" width="9.07421875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="14.6" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -728,8 +806,11 @@
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="6">
         <v>3.8</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -751,9 +832,10 @@
       <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="6">
         <v>35</v>
       </c>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1">
@@ -774,9 +856,10 @@
       <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="6">
         <v>4</v>
       </c>
+      <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1">
@@ -797,9 +880,10 @@
       <c r="F5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="6">
         <v>3.8</v>
       </c>
+      <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1">
@@ -820,9 +904,10 @@
       <c r="F6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="6">
         <v>35</v>
       </c>
+      <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1">
@@ -843,9 +928,10 @@
       <c r="F7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="6">
         <v>4</v>
       </c>
+      <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1">
@@ -866,11 +952,12 @@
       <c r="F8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="6">
         <v>16.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" ht="14.6" thickBot="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -889,9 +976,10 @@
       <c r="F9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="6">
         <v>0.33</v>
       </c>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1">
@@ -1016,25 +1104,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G15" s="5">
         <v>8000</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1058,7 +1146,7 @@
       </c>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:13">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1079,7 +1167,7 @@
       </c>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:13">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1102,24 +1190,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:13">
       <c r="I19" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:13">
       <c r="I20" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="I21" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="I22" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="I22" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
big improvement: list below
1. print more cfar details;
2. disable the sysview;
3. speedup the fast sample rate;
4. add warm-cool color control;
5. remove the dead section delay;
6. fix T=4.8s slow check;
7. add hand wave func;
8. optimise the show check logic;
9. optimise the sense delay check;
10. add light_sensor2 debug info;
11. add beeper i/o.
</commit_message>
<xml_diff>
--- a/DOC/flash分配.xlsx
+++ b/DOC/flash分配.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="16157" windowHeight="8503"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="16155" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -748,23 +748,23 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.69140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.23046875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.921875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.69140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.15234375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.53515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.23046875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.69140625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.07421875" style="2"/>
+    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.19921875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.9296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.1328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.53125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.19921875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.6" thickBot="1">
+    <row r="1" spans="1:8" ht="13.9" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -806,9 +806,7 @@
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="6">
-        <v>3.8</v>
-      </c>
+      <c r="G2" s="6"/>
       <c r="H2" s="7" t="s">
         <v>70</v>
       </c>
@@ -832,9 +830,7 @@
       <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="6">
-        <v>35</v>
-      </c>
+      <c r="G3" s="6"/>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8">
@@ -856,9 +852,7 @@
       <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="6">
-        <v>4</v>
-      </c>
+      <c r="G4" s="6"/>
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8">
@@ -880,9 +874,7 @@
       <c r="F5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="6">
-        <v>3.8</v>
-      </c>
+      <c r="G5" s="6"/>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8">
@@ -904,9 +896,7 @@
       <c r="F6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="6">
-        <v>35</v>
-      </c>
+      <c r="G6" s="6"/>
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8">
@@ -928,9 +918,7 @@
       <c r="F7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="6">
-        <v>4</v>
-      </c>
+      <c r="G7" s="6"/>
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8">
@@ -952,12 +940,10 @@
       <c r="F8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="6">
-        <v>16.5</v>
-      </c>
+      <c r="G8" s="6"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:8" ht="14.6" thickBot="1">
+    <row r="9" spans="1:8" ht="13.9" thickBot="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -976,9 +962,7 @@
       <c r="F9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="6">
-        <v>0.33</v>
-      </c>
+      <c r="G9" s="6"/>
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8">
@@ -1070,7 +1054,7 @@
         <v>45</v>
       </c>
       <c r="G13" s="5">
-        <v>3800</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1093,7 +1077,7 @@
         <v>58</v>
       </c>
       <c r="G14" s="5">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
fix two bugs: list below
1. onboard led en/disable;
2. load parameter flash save and restore
</commit_message>
<xml_diff>
--- a/DOC/flash分配.xlsx
+++ b/DOC/flash分配.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="16157" windowHeight="8503"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="16155" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
   <si>
     <t>全局变量</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -293,6 +293,22 @@
   </si>
   <si>
     <t>protocol.c:reset_default_parameter()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>load_radar_parameter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加载覆盖范围</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x38</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -745,26 +761,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.69140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.23046875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.921875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.69140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.15234375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.53515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.23046875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.69140625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.07421875" style="2"/>
+    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.19921875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.9296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.1328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.53125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.19921875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.6" thickBot="1">
+    <row r="1" spans="1:8" ht="13.9" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -806,9 +822,7 @@
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="6">
-        <v>3.8</v>
-      </c>
+      <c r="G2" s="6"/>
       <c r="H2" s="7" t="s">
         <v>70</v>
       </c>
@@ -832,9 +846,7 @@
       <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="6">
-        <v>35</v>
-      </c>
+      <c r="G3" s="6"/>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8">
@@ -856,9 +868,7 @@
       <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="6">
-        <v>4</v>
-      </c>
+      <c r="G4" s="6"/>
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8">
@@ -880,9 +890,7 @@
       <c r="F5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="6">
-        <v>3.8</v>
-      </c>
+      <c r="G5" s="6"/>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8">
@@ -904,9 +912,7 @@
       <c r="F6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="6">
-        <v>35</v>
-      </c>
+      <c r="G6" s="6"/>
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8">
@@ -928,9 +934,7 @@
       <c r="F7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="6">
-        <v>4</v>
-      </c>
+      <c r="G7" s="6"/>
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8">
@@ -952,12 +956,10 @@
       <c r="F8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="6">
-        <v>16.5</v>
-      </c>
+      <c r="G8" s="6"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:8" ht="14.6" thickBot="1">
+    <row r="9" spans="1:8" ht="13.9" thickBot="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -976,9 +978,7 @@
       <c r="F9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="6">
-        <v>0.33</v>
-      </c>
+      <c r="G9" s="6"/>
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8">
@@ -1130,40 +1130,42 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="G16" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G17" s="5"/>
     </row>
@@ -1172,44 +1174,65 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="E19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G19" s="5">
         <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="I19" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="I20" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="I21" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="I22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="I23" s="2" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix two bugs: 1. onboard led en/disable; 2. load parameter flash save and restore
</commit_message>
<xml_diff>
--- a/DOC/flash分配.xlsx
+++ b/DOC/flash分配.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="16157" windowHeight="8503"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="16155" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
   <si>
     <t>全局变量</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -293,6 +293,22 @@
   </si>
   <si>
     <t>protocol.c:reset_default_parameter()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>load_radar_parameter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加载覆盖范围</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x38</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -745,26 +761,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.69140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.23046875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.921875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.69140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.15234375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.53515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.23046875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.69140625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.07421875" style="2"/>
+    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.19921875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.9296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.1328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.53125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.19921875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.6" thickBot="1">
+    <row r="1" spans="1:8" ht="13.9" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -806,9 +822,7 @@
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="6">
-        <v>3.8</v>
-      </c>
+      <c r="G2" s="6"/>
       <c r="H2" s="7" t="s">
         <v>70</v>
       </c>
@@ -832,9 +846,7 @@
       <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="6">
-        <v>35</v>
-      </c>
+      <c r="G3" s="6"/>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8">
@@ -856,9 +868,7 @@
       <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="6">
-        <v>4</v>
-      </c>
+      <c r="G4" s="6"/>
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8">
@@ -880,9 +890,7 @@
       <c r="F5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="6">
-        <v>3.8</v>
-      </c>
+      <c r="G5" s="6"/>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8">
@@ -904,9 +912,7 @@
       <c r="F6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="6">
-        <v>35</v>
-      </c>
+      <c r="G6" s="6"/>
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8">
@@ -928,9 +934,7 @@
       <c r="F7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="6">
-        <v>4</v>
-      </c>
+      <c r="G7" s="6"/>
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8">
@@ -952,12 +956,10 @@
       <c r="F8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="6">
-        <v>16.5</v>
-      </c>
+      <c r="G8" s="6"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:8" ht="14.6" thickBot="1">
+    <row r="9" spans="1:8" ht="13.9" thickBot="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -976,9 +978,7 @@
       <c r="F9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="6">
-        <v>0.33</v>
-      </c>
+      <c r="G9" s="6"/>
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8">
@@ -1130,40 +1130,42 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="G16" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G17" s="5"/>
     </row>
@@ -1172,44 +1174,65 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="E19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G19" s="5">
         <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="I19" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="I20" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="I21" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="I22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="I23" s="2" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>